<commit_message>
refract and complete <el-option>, update .gitignore
</commit_message>
<xml_diff>
--- a/document/info/Race.xlsx
+++ b/document/info/Race.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0_Personal_File\Database\db_project\document\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E804B10-5252-4D5A-866E-08A6DB196634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D95F728-9886-4ACF-BB78-62D0456895A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
   <si>
     <t>龙</t>
   </si>
@@ -423,7 +423,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -712,15 +712,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -736,8 +736,14 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -749,8 +755,14 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -762,8 +774,14 @@
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -775,8 +793,14 @@
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>97</v>
       </c>
@@ -788,8 +812,14 @@
       <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -801,8 +831,14 @@
       <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -814,8 +850,14 @@
       <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>96</v>
       </c>
@@ -827,8 +869,14 @@
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -844,8 +892,14 @@
       <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="18.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -857,8 +911,14 @@
       <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -870,8 +930,14 @@
       <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
@@ -887,8 +953,14 @@
       <c r="E12" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -900,8 +972,14 @@
       <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -917,8 +995,14 @@
       <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -930,8 +1014,14 @@
       <c r="E15" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
@@ -943,8 +1033,14 @@
       <c r="E16" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -960,8 +1056,14 @@
       <c r="E17" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -977,8 +1079,14 @@
       <c r="E18" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
@@ -994,8 +1102,14 @@
       <c r="E19" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>54</v>
       </c>
@@ -1011,8 +1125,14 @@
       <c r="E20" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
@@ -1024,8 +1144,14 @@
       <c r="E21" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
@@ -1037,8 +1163,14 @@
       <c r="E22" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>63</v>
       </c>
@@ -1051,7 +1183,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>66</v>
       </c>
@@ -1068,7 +1200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -1081,7 +1213,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
@@ -1094,7 +1226,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>74</v>
       </c>
@@ -1107,7 +1239,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>77</v>
       </c>
@@ -1120,7 +1252,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>80</v>
       </c>
@@ -1137,7 +1269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>82</v>
       </c>
@@ -1150,7 +1282,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>85</v>
       </c>
@@ -1163,7 +1295,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
@@ -1176,7 +1308,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>90</v>
       </c>
@@ -1189,7 +1321,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>93</v>
       </c>
@@ -1198,7 +1330,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>94</v>
       </c>
@@ -1207,7 +1339,7 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>95</v>
       </c>

</xml_diff>